<commit_message>
Add Database Utility and modify Excel Utility
</commit_message>
<xml_diff>
--- a/TestData/empdata.xlsx
+++ b/TestData/empdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6902f846743b03e3/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\DbExcelCompare\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{CC910892-4B2B-4980-A53F-1EF15829AE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74C5A41A-C2C1-4CEE-9A7E-1E75581EA0CC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4450EC7-597C-4B6A-99FE-F74BC54C76FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{9283304F-8988-47A3-9584-A7DFC195C58C}"/>
+    <workbookView xWindow="5280" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{9283304F-8988-47A3-9584-A7DFC195C58C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Chavanke</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20F66DF-6E0D-4DAD-8003-B8504E5A5AF3}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -487,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>40000</v>
+        <v>24000</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -518,7 +523,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1">
         <v>40000</v>

</xml_diff>